<commit_message>
Further description of process models
</commit_message>
<xml_diff>
--- a/ProM/Process_Model_Creation/ProM_Model_Input_Values_New.xlsx
+++ b/ProM/Process_Model_Creation/ProM_Model_Input_Values_New.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEVMEYE3\Documents\Master\BPI Challenge 2019\New_Exports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince_000\Documents\GitHub\BPI_Challenge_2019\ProM\Process_Model_Creation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6167043-31EA-48FF-A13F-C93CB4F14C20}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12780" yWindow="2730" windowWidth="21600" windowHeight="11010"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New" sheetId="1" r:id="rId1"/>
-    <sheet name="Archive" sheetId="2" r:id="rId2"/>
+    <sheet name="Detailed_02_02_01" sheetId="3" r:id="rId2"/>
+    <sheet name="Archive" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="CIQWBGuid" hidden="1">"8f944a8e-e448-477a-8bf8-39d9299f8220"</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>Cluster</t>
   </si>
@@ -220,12 +223,15 @@
   </si>
   <si>
     <t>02_01</t>
+  </si>
+  <si>
+    <t>02_02_01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -630,29 +636,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="50.68359375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.05078125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -666,34 +667,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>33</v>
       </c>
@@ -707,34 +693,19 @@
         <v>7651</v>
       </c>
       <c r="E2">
-        <v>90</v>
+        <v>303</v>
       </c>
       <c r="F2">
-        <v>90</v>
+        <v>6975</v>
       </c>
       <c r="G2">
-        <v>90</v>
+        <v>87.3</v>
       </c>
       <c r="H2">
-        <v>303</v>
-      </c>
-      <c r="I2">
-        <v>6975</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2">
-        <v>0.2</v>
-      </c>
-      <c r="L2">
-        <v>87.3</v>
-      </c>
-      <c r="M2">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
         <v>48</v>
       </c>
@@ -748,34 +719,19 @@
         <v>1163</v>
       </c>
       <c r="E3">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="F3">
-        <v>80</v>
+        <v>1158</v>
       </c>
       <c r="G3">
-        <v>90</v>
+        <v>95.8</v>
       </c>
       <c r="H3">
-        <v>96</v>
-      </c>
-      <c r="I3">
-        <v>1158</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3">
-        <v>0.2</v>
-      </c>
-      <c r="L3">
-        <v>95.8</v>
-      </c>
-      <c r="M3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8" t="s">
         <v>34</v>
       </c>
@@ -789,34 +745,19 @@
         <v>10565</v>
       </c>
       <c r="E4">
-        <v>80</v>
+        <v>598</v>
       </c>
       <c r="F4">
-        <v>90</v>
+        <v>8045</v>
       </c>
       <c r="G4">
-        <v>90</v>
+        <v>91.4</v>
       </c>
       <c r="H4">
-        <v>598</v>
-      </c>
-      <c r="I4">
-        <v>8045</v>
-      </c>
-      <c r="J4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4">
-        <v>0.2</v>
-      </c>
-      <c r="L4">
-        <v>91.4</v>
-      </c>
-      <c r="M4">
         <v>61.5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8" t="s">
         <v>41</v>
       </c>
@@ -830,34 +771,19 @@
         <v>38101</v>
       </c>
       <c r="E5">
-        <v>90</v>
+        <v>6347</v>
       </c>
       <c r="F5">
-        <v>90</v>
+        <v>34529</v>
       </c>
       <c r="G5">
-        <v>90</v>
+        <v>94.3</v>
       </c>
       <c r="H5">
-        <v>6347</v>
-      </c>
-      <c r="I5">
-        <v>34529</v>
-      </c>
-      <c r="J5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>94.3</v>
-      </c>
-      <c r="M5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8" t="s">
         <v>42</v>
       </c>
@@ -871,34 +797,19 @@
         <v>1518</v>
       </c>
       <c r="E6">
-        <v>80</v>
+        <v>265</v>
       </c>
       <c r="F6">
-        <v>80</v>
+        <v>1366</v>
       </c>
       <c r="G6">
-        <v>80</v>
+        <v>94.1</v>
       </c>
       <c r="H6">
-        <v>265</v>
-      </c>
-      <c r="I6">
-        <v>1366</v>
-      </c>
-      <c r="J6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6">
-        <v>0.1</v>
-      </c>
-      <c r="L6">
-        <v>94.1</v>
-      </c>
-      <c r="M6">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="9" t="s">
         <v>61</v>
       </c>
@@ -912,295 +823,147 @@
         <v>8754</v>
       </c>
       <c r="E7">
-        <v>90</v>
+        <v>675</v>
       </c>
       <c r="F7">
-        <v>90</v>
+        <v>8225</v>
       </c>
       <c r="G7">
+        <v>94.7</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="8">
+        <v>161613</v>
+      </c>
+      <c r="D8">
+        <v>944234</v>
+      </c>
+      <c r="E8">
+        <v>158834</v>
+      </c>
+      <c r="F8">
+        <v>855021</v>
+      </c>
+      <c r="G8">
         <v>93</v>
       </c>
-      <c r="H7">
-        <v>675</v>
-      </c>
-      <c r="I7">
-        <v>8225</v>
-      </c>
-      <c r="J7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7">
-        <v>0.2</v>
-      </c>
-      <c r="L7">
-        <v>94.7</v>
-      </c>
-      <c r="M7">
+      <c r="H8">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="8">
-        <v>111487</v>
-      </c>
-      <c r="D8">
-        <v>594068</v>
-      </c>
-      <c r="E8">
-        <v>90</v>
-      </c>
-      <c r="F8">
-        <v>90</v>
-      </c>
-      <c r="G8">
-        <v>90</v>
-      </c>
-      <c r="H8">
-        <v>111487</v>
-      </c>
-      <c r="I8">
-        <v>557435</v>
-      </c>
-      <c r="J8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8">
-        <v>0.2</v>
-      </c>
-      <c r="L8">
-        <v>96.5</v>
-      </c>
-      <c r="M8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1611</v>
+      </c>
+      <c r="D9">
+        <v>12062</v>
+      </c>
+      <c r="E9">
+        <v>1534</v>
+      </c>
+      <c r="F9">
+        <v>10662</v>
+      </c>
+      <c r="G9">
+        <v>90.3</v>
+      </c>
+      <c r="H9">
+        <v>87.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="8">
+        <v>4167</v>
+      </c>
+      <c r="D10">
+        <v>23626</v>
+      </c>
+      <c r="E10">
+        <v>3964</v>
+      </c>
+      <c r="F10">
+        <v>21122</v>
+      </c>
+      <c r="G10">
+        <v>91.6</v>
+      </c>
+      <c r="H10">
+        <v>90.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="8">
+        <v>287</v>
+      </c>
+      <c r="D11">
+        <v>2364</v>
+      </c>
+      <c r="E11">
+        <v>258</v>
+      </c>
+      <c r="F11">
+        <v>2155</v>
+      </c>
+      <c r="G11">
+        <v>97.1</v>
+      </c>
+      <c r="H11">
+        <v>69.900000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="8">
+        <v>13397</v>
+      </c>
+      <c r="D12">
+        <v>33738</v>
+      </c>
+      <c r="E12">
+        <v>13128</v>
+      </c>
+      <c r="F12">
+        <v>30447</v>
+      </c>
+      <c r="G12">
+        <v>93.8</v>
+      </c>
+      <c r="H12">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="8">
-        <v>32087</v>
-      </c>
-      <c r="D9" s="8">
-        <v>205531</v>
-      </c>
-      <c r="E9">
-        <v>90</v>
-      </c>
-      <c r="F9">
-        <v>90</v>
-      </c>
-      <c r="G9">
-        <v>90</v>
-      </c>
-      <c r="H9">
-        <v>32087</v>
-      </c>
-      <c r="I9">
-        <v>188006</v>
-      </c>
-      <c r="L9">
-        <v>94.4</v>
-      </c>
-      <c r="M9">
-        <v>93.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="8">
-        <v>18039</v>
-      </c>
-      <c r="D10" s="8">
-        <v>146635</v>
-      </c>
-      <c r="H10">
-        <v>17337</v>
-      </c>
-      <c r="I10">
-        <v>129034</v>
-      </c>
-      <c r="L10">
-        <v>82.3</v>
-      </c>
-      <c r="M10">
-        <v>87.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="8">
-        <v>1611</v>
-      </c>
-      <c r="D11">
-        <v>12062</v>
-      </c>
-      <c r="E11">
-        <v>90</v>
-      </c>
-      <c r="F11">
-        <v>90</v>
-      </c>
-      <c r="G11">
-        <v>90</v>
-      </c>
-      <c r="H11">
-        <v>1534</v>
-      </c>
-      <c r="I11">
-        <v>10662</v>
-      </c>
-      <c r="J11" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11">
-        <v>0.2</v>
-      </c>
-      <c r="L11">
-        <v>90.3</v>
-      </c>
-      <c r="M11">
-        <v>87.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="8">
-        <v>4167</v>
-      </c>
-      <c r="D12">
-        <v>23626</v>
-      </c>
-      <c r="E12">
-        <v>90</v>
-      </c>
-      <c r="F12">
-        <v>90</v>
-      </c>
-      <c r="G12">
-        <v>90</v>
-      </c>
-      <c r="H12">
-        <v>3964</v>
-      </c>
-      <c r="I12">
-        <v>21122</v>
-      </c>
-      <c r="J12" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12">
-        <v>0.2</v>
-      </c>
-      <c r="L12">
-        <v>91.6</v>
-      </c>
-      <c r="M12">
-        <v>90.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="8">
-        <v>287</v>
-      </c>
-      <c r="D13">
-        <v>2364</v>
-      </c>
-      <c r="E13">
-        <v>90</v>
-      </c>
-      <c r="F13">
-        <v>90</v>
-      </c>
-      <c r="G13">
-        <v>90</v>
-      </c>
-      <c r="H13">
-        <v>258</v>
-      </c>
-      <c r="I13">
-        <v>2155</v>
-      </c>
-      <c r="J13" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13">
-        <v>0.3</v>
-      </c>
-      <c r="L13">
-        <v>97.1</v>
-      </c>
-      <c r="M13">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="8">
-        <v>13397</v>
-      </c>
-      <c r="D14">
-        <v>33738</v>
-      </c>
-      <c r="E14">
-        <v>90</v>
-      </c>
-      <c r="F14">
-        <v>90</v>
-      </c>
-      <c r="G14">
-        <v>90</v>
-      </c>
-      <c r="H14">
-        <v>13128</v>
-      </c>
-      <c r="I14">
-        <v>30447</v>
-      </c>
-      <c r="J14" t="s">
-        <v>9</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>93.8</v>
-      </c>
-      <c r="M14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="7"/>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C23" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1209,16 +972,139 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92D1811-F4A2-4C7D-A263-4FA5BDA43144}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="11.5234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.3671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.05078125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="8">
+        <v>111487</v>
+      </c>
+      <c r="D2">
+        <v>594068</v>
+      </c>
+      <c r="E2">
+        <v>111487</v>
+      </c>
+      <c r="F2">
+        <v>557435</v>
+      </c>
+      <c r="G2">
+        <v>96.5</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="8">
+        <v>32087</v>
+      </c>
+      <c r="D3" s="8">
+        <v>205531</v>
+      </c>
+      <c r="E3">
+        <v>32087</v>
+      </c>
+      <c r="F3">
+        <v>188006</v>
+      </c>
+      <c r="G3">
+        <v>94.4</v>
+      </c>
+      <c r="H3">
+        <v>93.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="8">
+        <v>18039</v>
+      </c>
+      <c r="D4" s="8">
+        <v>146635</v>
+      </c>
+      <c r="E4">
+        <v>17337</v>
+      </c>
+      <c r="F4">
+        <v>129034</v>
+      </c>
+      <c r="G4">
+        <v>82.3</v>
+      </c>
+      <c r="H4">
+        <v>87.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1259,7 +1145,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1294,7 +1180,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1335,7 +1221,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1352,7 +1238,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1393,7 +1279,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1410,7 +1296,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
@@ -1451,7 +1337,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -1492,7 +1378,7 @@
         <v>75.099999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1533,7 +1419,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1574,7 +1460,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1615,7 +1501,7 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>34</v>
       </c>

</xml_diff>